<commit_message>
Update firing order and pushrod adjustement.xlsx
</commit_message>
<xml_diff>
--- a/s-10/firing order and pushrod adjustement.xlsx
+++ b/s-10/firing order and pushrod adjustement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20385"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20387"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ORB User\Documents\GitHub\Stuff\s-10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB562C1-0C25-4C52-8612-F038B09F9D21}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC7892BB-64EE-4DF4-BDE4-A5F3EEDBFE9A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="3" xr2:uid="{998C4E01-B4A7-44CA-BFD6-90B60591AA22}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="2" xr2:uid="{998C4E01-B4A7-44CA-BFD6-90B60591AA22}"/>
   </bookViews>
   <sheets>
     <sheet name="pushrods" sheetId="1" r:id="rId1"/>
@@ -818,11 +818,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E4B3309-E840-4263-A4F2-8836BCCB9E4E}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -857,7 +860,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CACF1671-B624-4BFC-91C5-B54C2D1DEB51}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>